<commit_message>
fixed contract structure in swaps tests
</commit_message>
<xml_diff>
--- a/data/excel/actus-tests-swaps.xlsx
+++ b/data/excel/actus-tests-swaps.xlsx
@@ -108,7 +108,7 @@
     <t>RFL</t>
   </si>
   <si>
-    <t>[{"object":{"contractType":"PAM","contractID":"swap01-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1","premiumDiscountAtIED":"0"},"type":"CNT","role":"FIL"},{"object":{"contractType":"PAM","contractID":"swap01-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1200","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P3ML1","premiumDiscountAtIED":"0"},"type":"CNT","role":"SEL"}]</t>
+    <t>[{"object":{"contractType":"PAM","contractID":"swap01-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1","premiumDiscountAtIED":"0"},"referenceType":"CNT","referenceRole":"FIL"},{"object":{"contractType":"PAM","contractID":"swap01-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1200","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P3ML1","premiumDiscountAtIED":"0"},"referenceType":"CNT","referenceRole":"SEL"}]</t>
   </si>
   <si>
     <t>USD</t>
@@ -132,7 +132,7 @@
     <t>PFL</t>
   </si>
   <si>
-    <t>[{"object":{"contractType":"PAM","contractID":"swap02-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1","premiumDiscountAtIED":"0"},"type":"CNT","role":"FIL"},{"object":{"contractType":"PAM","contractID":"swap02-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1200","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfRateReset":"2013-02-01T00:00:00","cycleOfRateReset":"P3ML1","rateSpread":"0.02","marketObjectCodeOfRateReset":"US_TREASURY","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1","premiumDiscountAtIED":"-200"},"type":"CNT","role":"SEL"}]</t>
+    <t>[{"object":{"contractType":"PAM","contractID":"swap02-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1","premiumDiscountAtIED":"0"},"referenceType":"CNT","referenceRole":"FIL"},{"object":{"contractType":"PAM","contractID":"swap02-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1200","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfRateReset":"2013-02-01T00:00:00","cycleOfRateReset":"P3ML1","rateSpread":"0.02","marketObjectCodeOfRateReset":"US_TREASURY","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1","premiumDiscountAtIED":"-200"},"referenceType":"CNT","referenceRole":"SEL"}]</t>
   </si>
   <si>
     <t>{"US_TREASURY":{"identifier":"US_TREASURY","data":[{"timestamp":"2013-02-01T00:00:00","value":"0.009827160493827160"},{"timestamp":"2013-05-01T00:00:00","value":"0.010938271602981800"},{"timestamp":"2013-08-01T00:00:00","value":"0.012049382716049400"},{"timestamp":"2013-11-01T00:00:00","value":"0.013160493827160500"}]}}</t>
@@ -141,7 +141,7 @@
     <t>swap03</t>
   </si>
   <si>
-    <t>[{"object":{"contractType":"PAM","contractID":"swap03-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfRateReset":"2013-03-01T00:00:00","cycleOfRateReset":"P3ML1","rateSpread":"0.025","marketObjectCodeOfRateReset":"US_TREASURY","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1"},"type":"CNT","role":"FIL"},{"object":{"contractType":"PAM","contractID":"swap03-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1200","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfRateReset":"2013-02-01T00:00:00","cycleOfRateReset":"P3ML1","rateSpread":"0.02","marketObjectCodeOfRateReset":"USD_LIBOR","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1","premiumDiscountAtIED":"-200"},"type":"CNT","role":"SEL"}]</t>
+    <t>[{"object":{"contractType":"PAM","contractID":"swap03-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfRateReset":"2013-03-01T00:00:00","cycleOfRateReset":"P3ML1","rateSpread":"0.025","marketObjectCodeOfRateReset":"US_TREASURY","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1"},"referenceType":"CNT","referenceRole":"FIL"},{"object":{"contractType":"PAM","contractID":"swap03-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1200","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfRateReset":"2013-02-01T00:00:00","cycleOfRateReset":"P3ML1","rateSpread":"0.02","marketObjectCodeOfRateReset":"USD_LIBOR","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1","premiumDiscountAtIED":"-200"},"referenceType":"CNT","referenceRole":"SEL"}]</t>
   </si>
   <si>
     <t>{"US_TREASURY":{"identifier":"US_TREASURY","data":[{"timestamp":"2013-03-01T00:00:00","value":"0.01019753086419750"},{"timestamp":"2013-06-01T00:00:00","value":"0.01130864197410850"},{"timestamp":"2013-09-01T00:00:00","value":"0.01241975308641980"},{"timestamp":"2013-12-01T00:00:00","value":"0.01353086419753090"}]},"USD_LIBOR":{"identifier":"USD_LIBOR","data":[{"timestamp":"2013-02-01T00:00:00","value":"0.0098271604945178"},{"timestamp":"2013-05-01T00:00:00","value":"0.0109382716029818"},{"timestamp":"2013-08-01T00:00:00","value":"0.0120493827160494"},{"timestamp":"2013-11-01T00:00:00","value":"0.0131604938271605"}]}}</t>
@@ -150,13 +150,13 @@
     <t>swap04</t>
   </si>
   <si>
-    <t>[{"object":{"contractType":"ANN","contractID":"swap04-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"6000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfInterestPayment":"2013-04-01T00:00:00","cycleOfInterestPayment":"P3ML1","cycleAnchorDateOfPrincipalRedemption":"2013-02-01T00:00:00","cycleOfPrincipalRedemption":"P1ML0","amortizationDate":"2013-12-15T00:00:00"},"type":"CNT","role":"FIL"},{"object":{"contractType":"ANN","contractID":"swap04-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"5000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfInterestPayment":"2013-04-01T00:00:00","cycleOfInterestPayment":"P3ML1","cycleAnchorDateOfPrincipalRedemption":"2013-04-01T00:00:00","cycleOfPrincipalRedemption":"P3ML1","amortizationDate":"2014-01-01T00:00:00"},"type":"CNT","role":"SEL"}]</t>
+    <t>[{"object":{"contractType":"ANN","contractID":"swap04-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"6000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfInterestPayment":"2013-04-01T00:00:00","cycleOfInterestPayment":"P3ML1","cycleAnchorDateOfPrincipalRedemption":"2013-02-01T00:00:00","cycleOfPrincipalRedemption":"P1ML0","amortizationDate":"2013-12-15T00:00:00"},"referenceType":"CNT","referenceRole":"FIL"},{"object":{"contractType":"ANN","contractID":"swap04-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"5000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfInterestPayment":"2013-04-01T00:00:00","cycleOfInterestPayment":"P3ML1","cycleAnchorDateOfPrincipalRedemption":"2013-04-01T00:00:00","cycleOfPrincipalRedemption":"P3ML1","amortizationDate":"2014-01-01T00:00:00"},"referenceType":"CNT","referenceRole":"SEL"}]</t>
   </si>
   <si>
     <t>swap05</t>
   </si>
   <si>
-    <t>[{"object":{"contractType":"ANN","contractID":"swap05-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"6000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfInterestPayment":"2013-02-01T00:00:00","cycleOfInterestPayment":"P1ML0","cycleAnchorDateOfPrincipalRedemption":"2013-02-01T00:00:00","cycleOfPrincipalRedemption":"P1ML0","amortizationDate":"2013-12-15T00:00:00"},"type":"CNT","role":"FIL"},{"object":{"contractType":"ANN","contractID":"swap05-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"5000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfRateReset":"2013-04-01T00:00:00","cycleOfRateReset":"P3ML1","rateSpread":"0.1","marketObjectCodeOfRateReset":"US_TREASURY","cycleAnchorDateOfInterestPayment":"2013-03-01T00:00:00","cycleOfInterestPayment":"P1ML0","cycleAnchorDateOfPrincipalRedemption":"2013-03-01T00:00:00","cycleOfPrincipalRedemption":"P1ML0","amortizationDate":"2014-01-01T00:00:00"},"type":"CNT","role":"SEL"}]</t>
+    <t>[{"object":{"contractType":"ANN","contractID":"swap05-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"6000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfInterestPayment":"2013-02-01T00:00:00","cycleOfInterestPayment":"P1ML0","cycleAnchorDateOfPrincipalRedemption":"2013-02-01T00:00:00","cycleOfPrincipalRedemption":"P1ML0","amortizationDate":"2013-12-15T00:00:00"},"referenceType":"CNT","referenceRole":"FIL"},{"object":{"contractType":"ANN","contractID":"swap05-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"5000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfRateReset":"2013-04-01T00:00:00","cycleOfRateReset":"P3ML1","rateSpread":"0.1","marketObjectCodeOfRateReset":"US_TREASURY","cycleAnchorDateOfInterestPayment":"2013-03-01T00:00:00","cycleOfInterestPayment":"P1ML0","cycleAnchorDateOfPrincipalRedemption":"2013-03-01T00:00:00","cycleOfPrincipalRedemption":"P1ML0","amortizationDate":"2014-01-01T00:00:00"},"referenceType":"CNT","referenceRole":"SEL"}]</t>
   </si>
   <si>
     <t>{"US_TREASURY":{"identifier":"US_TREASURY","data":[{"timestamp":"2013-04-01T00:00:00","value":"0.01056790123234830"},{"timestamp":"2013-07-01T00:00:00","value":"0.01167901234567900"},{"timestamp":"2013-10-01T00:00:00","value":"0.01279012345679010"}]}}</t>
@@ -165,7 +165,7 @@
     <t>swap06</t>
   </si>
   <si>
-    <t>[{"object":{"contractType":"ANN","contractID":"swap06-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"6000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfRateReset":"2013-04-01T00:00:00","cycleOfRateReset":"P3ML1","rateSpread":"0.1","marketObjectCodeOfRateReset":"US_TREASURY","cycleAnchorDateOfInterestPayment":"2013-03-01T00:00:00","cycleOfInterestPayment":"P1ML0","cycleAnchorDateOfPrincipalRedemption":"2013-03-01T00:00:00","cycleOfPrincipalRedemption":"P1ML0","amortizationDate":"2014-01-01T00:00:00"},"type":"CNT","role":"FIL"},{"object":{"contractType":"ANN","contractID":"swap06-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"5000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfRateReset":"2013-04-01T00:00:00","cycleOfRateReset":"P4ML1","rateSpread":"0.1","marketObjectCodeOfRateReset":"USD_LIBOR","cycleAnchorDateOfInterestPayment":"2013-03-01T00:00:00","cycleOfInterestPayment":"P2ML0","cycleAnchorDateOfPrincipalRedemption":"2013-03-01T00:00:00","cycleOfPrincipalRedemption":"P2ML0","amortizationDate":"2014-01-01T00:00:00"},"type":"CNT","role":"SEL"}]</t>
+    <t>[{"object":{"contractType":"ANN","contractID":"swap06-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"6000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfRateReset":"2013-04-01T00:00:00","cycleOfRateReset":"P3ML1","rateSpread":"0.1","marketObjectCodeOfRateReset":"US_TREASURY","cycleAnchorDateOfInterestPayment":"2013-03-01T00:00:00","cycleOfInterestPayment":"P1ML0","cycleAnchorDateOfPrincipalRedemption":"2013-03-01T00:00:00","cycleOfPrincipalRedemption":"P1ML0","amortizationDate":"2014-01-01T00:00:00"},"referenceType":"CNT","referenceRole":"FIL"},{"object":{"contractType":"ANN","contractID":"swap06-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"5000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfRateReset":"2013-04-01T00:00:00","cycleOfRateReset":"P4ML1","rateSpread":"0.1","marketObjectCodeOfRateReset":"USD_LIBOR","cycleAnchorDateOfInterestPayment":"2013-03-01T00:00:00","cycleOfInterestPayment":"P2ML0","cycleAnchorDateOfPrincipalRedemption":"2013-03-01T00:00:00","cycleOfPrincipalRedemption":"P2ML0","amortizationDate":"2014-01-01T00:00:00"},"referenceType":"CNT","referenceRole":"SEL"}]</t>
   </si>
   <si>
     <t>{"US_TREASURY":{"identifier":"US_TREASURY","data":[{"timestamp":"2013-04-01T00:00:00","value":"0.010567901234567901"},{"timestamp":"2013-07-01T00:00:00","value":"0.011679012345679012"},{"timestamp":"2013-10-01T00:00:00","value":"0.012790123456790127"}]},"USD_LIBOR":{"identifier":"USD_LIBOR","data":[{"timestamp":"2013-04-01T00:00:00","value":"0.010753086419753085"},{"timestamp":"2013-08-01T00:00:00","value":"0.01223456790123457"},{"timestamp":"2013-12-01T00:00:00","value":"0.013716049382716054"}]}}</t>
@@ -174,13 +174,13 @@
     <t>swap07</t>
   </si>
   <si>
-    <t>[{"object":{"contractType":"PAM","contractID":"swap07-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1"},"type":"CNT","role":"FIL"},{"object":{"contractType":"ANN","contractID":"swap07-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"6000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfInterestPayment":"2013-02-01T00:00:00","cycleOfInterestPayment":"P1ML0","cycleAnchorDateOfPrincipalRedemption":"2013-02-01T00:00:00","cycleOfPrincipalRedemption":"P1ML0","amortizationDate":"2013-12-15T00:00:00"},"type":"CNT","role":"SEL"}]</t>
+    <t>[{"object":{"contractType":"PAM","contractID":"swap07-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1"},"referenceType":"CNT","referenceRole":"FIL"},{"object":{"contractType":"ANN","contractID":"swap07-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"6000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfInterestPayment":"2013-02-01T00:00:00","cycleOfInterestPayment":"P1ML0","cycleAnchorDateOfPrincipalRedemption":"2013-02-01T00:00:00","cycleOfPrincipalRedemption":"P1ML0","amortizationDate":"2013-12-15T00:00:00"},"referenceType":"CNT","referenceRole":"SEL"}]</t>
   </si>
   <si>
     <t>swap08</t>
   </si>
   <si>
-    <t>[{"object":{"contractType":"PAM","contractID":"swap08-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfRateReset":"2013-03-01T00:00:00","cycleOfRateReset":"P3ML1","rateSpread":"0.02","marketObjectCodeOfRateReset":"US_TREASURY","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1"},"type":"CNT","role":"FIL"},{"object":{"contractType":"ANN","contractID":"swap08-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"6000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfRateReset":"2013-04-01T00:00:00","cycleOfRateReset":"P3ML1","rateSpread":"0.1","marketObjectCodeOfRateReset":"USD_LIBOR","cycleAnchorDateOfInterestPayment":"2013-03-01T00:00:00","cycleOfInterestPayment":"P1ML0","cycleAnchorDateOfPrincipalRedemption":"2013-03-01T00:00:00","cycleOfPrincipalRedemption":"P1ML0","amortizationDate":"2014-01-01T00:00:00"},"type":"CNT","role":"SEL"}]</t>
+    <t>[{"object":{"contractType":"PAM","contractID":"swap08-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfRateReset":"2013-03-01T00:00:00","cycleOfRateReset":"P3ML1","rateSpread":"0.02","marketObjectCodeOfRateReset":"US_TREASURY","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1"},"referenceType":"CNT","referenceRole":"FIL"},{"object":{"contractType":"ANN","contractID":"swap08-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"6000","dayCountConvention":"A365","nominalInterestRate":"0.08","cycleAnchorDateOfRateReset":"2013-04-01T00:00:00","cycleOfRateReset":"P3ML1","rateSpread":"0.1","marketObjectCodeOfRateReset":"USD_LIBOR","cycleAnchorDateOfInterestPayment":"2013-03-01T00:00:00","cycleOfInterestPayment":"P1ML0","cycleAnchorDateOfPrincipalRedemption":"2013-03-01T00:00:00","cycleOfPrincipalRedemption":"P1ML0","amortizationDate":"2014-01-01T00:00:00"},"referenceType":"CNT","referenceRole":"SEL"}]</t>
   </si>
   <si>
     <t>{"US_TREASURY":{"identifier":"US_TREASURY","data":[{"timestamp":"2013-03-01T00:00:00","value":"0.010197530864197533"},{"timestamp":"2013-06-01T00:00:00","value":"0.011308641975308642"},{"timestamp":"2013-09-01T00:00:00","value":"0.012419753086419752"},{"timestamp":"2013-12-01T00:00:00","value":"0.013530864197530865"}]},"USD_LIBOR":{"identifier":"USD_LIBOR","data":[{"timestamp":"2013-04-01T00:00:00","value":"0.010567901234567901"},{"timestamp":"2013-07-01T00:00:00","value":"0.011679012345679012"},{"timestamp":"2013-10-01T00:00:00","value":"0.012790123456790127"}]}}</t>
@@ -189,7 +189,7 @@
     <t>swap09</t>
   </si>
   <si>
-    <t>[{"object":{"contractType":"PAM","contractID":"swap09-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1"},"type":"CNT","role":"FIL"},{"object":{"contractType":"PAM","contractID":"swap09-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1200","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P3ML1"},"type":"CNT","role":"SEL"}]</t>
+    <t>[{"object":{"contractType":"PAM","contractID":"swap09-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1"},"referenceType":"CNT","referenceRole":"FIL"},{"object":{"contractType":"PAM","contractID":"swap09-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1200","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P3ML1"},"referenceType":"CNT","referenceRole":"SEL"}]</t>
   </si>
   <si>
     <t>2013-03-15T23:59:59</t>
@@ -198,7 +198,7 @@
     <t>swap10</t>
   </si>
   <si>
-    <t>[{"object":{"contractType":"PAM","contractID":"swap10-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1"},"type":"CNT","role":"FIL"},{"object":{"contractType":"PAM","contractID":"swap10-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1200","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P3ML1"},"type":"CNT","role":"SEL"}]</t>
+    <t>[{"object":{"contractType":"PAM","contractID":"swap10-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1"},"referenceType":"CNT","referenceRole":"FIL"},{"object":{"contractType":"PAM","contractID":"swap10-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1200","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P3ML1"},"referenceType":"CNT","referenceRole":"SEL"}]</t>
   </si>
   <si>
     <t>2013-07-01T00:00:00</t>
@@ -207,7 +207,7 @@
     <t>swap11</t>
   </si>
   <si>
-    <t>[{"object":{"contractType":"PAM","contractID":"swap11-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1"},"type":"CNT","role":"FIL"},{"object":{"contractType":"PAM","contractID":"swap11-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1200","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P3ML1"},"type":"CNT","role":"SEL"}]</t>
+    <t>[{"object":{"contractType":"PAM","contractID":"swap11-leg1","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1000","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P1ML1"},"referenceType":"CNT","referenceRole":"FIL"},{"object":{"contractType":"PAM","contractID":"swap11-leg2","contractDealDate":"2012-12-28T00:00:00","initialExchangeDate":"2013-01-01T00:00:00","currency":"USD","statusDate":"2012-12-30T00:00:00","notionalPrincipal":"1200","dayCountConvention":"A365","nominalInterestRate":"0.1","maturityDate":"2014-01-01T00:00:00","cycleAnchorDateOfInterestPayment":"2013-01-01T00:00:00","cycleOfInterestPayment":"P3ML1"},"referenceType":"CNT","referenceRole":"SEL"}]</t>
   </si>
   <si>
     <t>S</t>

</xml_diff>